<commit_message>
updated images and finished events page
</commit_message>
<xml_diff>
--- a/docs/Session 5 2021 Schedule.xlsx
+++ b/docs/Session 5 2021 Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E59F9C9-AFA0-49A2-A368-8E396ED90E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78A6A2B-A452-49ED-9DF2-85C4070BAAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07DE24DF-01C4-4D74-B465-B843338AAF83}"/>
+    <workbookView xWindow="11115" yWindow="2685" windowWidth="28770" windowHeight="15570" xr2:uid="{07DE24DF-01C4-4D74-B465-B843338AAF83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>Pricing per 8 week session</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Mini Cats (Parent &amp; tot)</t>
   </si>
   <si>
-    <t>Mini Cats (walking- 3yrs)</t>
-  </si>
-  <si>
     <t>50 Min</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Tumbling</t>
   </si>
   <si>
-    <t>Tumble Cats</t>
-  </si>
-  <si>
     <t>Exhibition</t>
   </si>
   <si>
@@ -190,6 +184,18 @@
   </si>
   <si>
     <t xml:space="preserve">Special Needs </t>
+  </si>
+  <si>
+    <t>Tumble Cats (4 &amp; 5 yr olds)</t>
+  </si>
+  <si>
+    <t>30 Minutes</t>
+  </si>
+  <si>
+    <t>Tumble Cats(6-18 years old)</t>
+  </si>
+  <si>
+    <t>Mini Cats (walking- 2yrs)</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +241,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -256,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -336,12 +349,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -384,9 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,6 +440,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -431,6 +467,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -455,14 +497,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1391107</xdr:colOff>
+      <xdr:colOff>1400632</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>91757</xdr:rowOff>
+      <xdr:rowOff>63182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>895349</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:colOff>904874</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -486,7 +528,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6105982" y="4578032"/>
+          <a:off x="6134557" y="4549457"/>
           <a:ext cx="2333167" cy="1956118"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -796,15 +838,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB80A1C-1FFF-48B5-A789-CB5DCB0E01DC}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="6" width="8.7109375" customWidth="1"/>
     <col min="7" max="7" width="2.5703125" customWidth="1"/>
     <col min="8" max="8" width="25.28515625" customWidth="1"/>
@@ -813,19 +855,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="H1" s="30" t="s">
+      <c r="A1" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="H1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -862,16 +904,18 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4">
+      <c r="F3" s="39">
         <v>0.25</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="J3" s="6">
         <v>100</v>
@@ -885,10 +929,10 @@
       <c r="E4" s="7"/>
       <c r="F4" s="4"/>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="8">
         <v>100</v>
@@ -896,28 +940,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="9">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="38">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D5" s="10">
-        <v>0.20833333333333334</v>
+      <c r="D5" s="38">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="E5" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="F5" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F5" s="38">
         <v>0.16666666666666666</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="6">
         <v>100</v>
@@ -930,65 +974,67 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="E6" s="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F6" s="10">
-        <v>0.25</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="J6" s="8">
         <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="38">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C7" s="4">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.20833333333333334</v>
-      </c>
+      <c r="E7" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="F7" s="10"/>
       <c r="H7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="6">
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="C8" s="4">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.25</v>
+      </c>
       <c r="E8" s="4">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F8" s="4"/>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="8">
         <v>120</v>
@@ -998,479 +1044,510 @@
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
-        <v>0.29166666666666669</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="H9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="J9" s="6">
         <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="H10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C10" s="10">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D10" s="10">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="J10" s="13">
         <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C11" s="38">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D11" s="38">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E11" s="38">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="10">
         <v>0.25</v>
       </c>
-      <c r="D11" s="10">
+      <c r="C12" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="10">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="H11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="16">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="E12" s="10">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="39">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C12" s="4">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C13" s="4">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D13" s="39">
         <v>0.25</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="H12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="8">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="H13" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J13" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="31">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="10">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10">
         <v>0.27083333333333331</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="38">
         <v>0.25</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="8">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="10">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="H15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="16">
+        <v>15</v>
+      </c>
+      <c r="J15" s="6">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="H16" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="H16" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="32">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="H17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
+      <c r="H17" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="H18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10">
+        <v>0.27083333333333331</v>
+      </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="F23" s="10">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="4">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-    </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="10">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0.25</v>
+      </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="18" t="s">
+        <v>52</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4">
+        <v>0.22916666666666666</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10">
-        <v>0.3125</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="J30" s="18"/>
-    </row>
-    <row r="31" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="J31" s="18"/>
-    </row>
-    <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="31" t="s">
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="J31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="J32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
+    </row>
+    <row r="34" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25"/>
+      <c r="I37" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="4">
-        <v>0.3125</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="24" t="s">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
-      <c r="I36" t="s">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="I38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="I37" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="D39" s="26"/>
+      <c r="E39" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27" t="s">
+      <c r="F39" s="26"/>
+      <c r="I39" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27" t="s">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="27"/>
-      <c r="I38" s="28" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F39" s="9"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A33:F33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I38" r:id="rId1" xr:uid="{0F196279-4D2E-4D01-8E0D-96E621D02EE7}"/>
+    <hyperlink ref="I39" r:id="rId1" xr:uid="{0F196279-4D2E-4D01-8E0D-96E621D02EE7}"/>
   </hyperlinks>
-  <pageMargins left="0.1" right="0.1" top="0.35" bottom="0" header="0.3" footer="0.3"/>
+  <pageMargins left="0.1" right="0.1" top="0.3" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>